<commit_message>
updated resnet eval values
</commit_message>
<xml_diff>
--- a/model_evaluation_results.xlsx
+++ b/model_evaluation_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ville\Projects\adversarial_examples\coco_foolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C370A-DD94-41B3-AD5A-2F0F4C07DF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9428C7-E685-4FFF-9CEA-EE34353EF4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0F83A952-5D0A-4F73-9DF0-E8AC08021A47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0F83A952-5D0A-4F73-9DF0-E8AC08021A47}"/>
   </bookViews>
   <sheets>
     <sheet name="List of models" sheetId="4" r:id="rId1"/>
@@ -583,7 +583,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -681,7 +681,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -692,6 +691,16 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4284,338 +4293,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.13800000000000001</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.11</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.11</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.17599999999999999</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.112</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>9.4E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.22800000000000001</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.19</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.185</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.29699999999999999</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.20399999999999999</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.19900000000000001</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.17100000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.14099999999999999</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.112</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.111</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.17699999999999999</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.115</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.111</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>5.5E-2</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>0.02</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.20899999999999999</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.17699999999999999</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.17799999999999999</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.245</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.157</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.154</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.24199999999999999</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.16400000000000001</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.17399999999999999</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.33900000000000002</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.32100000000000001</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.23899999999999999</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.17599999999999999</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.151</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.152</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.189</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.151</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.14399999999999999</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.28499999999999998</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.248</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.25</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.29099999999999998</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.23499999999999999</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.22600000000000001</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.217</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.29699999999999999</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.26300000000000001</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.311</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.248</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.24299999999999999</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.23200000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.153</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.14899999999999999</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.13500000000000001</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.16</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.107</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.39900000000000002</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.34699999999999998</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.36199999999999999</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.42</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.36299999999999999</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.34699999999999998</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.499</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.37</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.54600000000000004</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.56699999999999995</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.39900000000000002</v>
       </c>
     </row>
@@ -4654,338 +4663,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.20599999999999999</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.16900000000000001</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.16500000000000001</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.24199999999999999</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.16300000000000001</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.16</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>0.154</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.32600000000000001</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.27100000000000002</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.39300000000000002</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.28100000000000003</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.27700000000000002</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.216</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.249</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.16400000000000001</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.16300000000000001</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.154</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>0.09</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>0.06</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.30399999999999999</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.26400000000000001</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.33800000000000002</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.22</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.224</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.21299999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.36</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.25</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.25600000000000001</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.44500000000000001</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.43</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.26900000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.22600000000000001</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.19800000000000001</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.19500000000000001</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.23499999999999999</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.189</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.18</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.183</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.36</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.32500000000000001</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.315</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.35899999999999999</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.28799999999999998</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.28100000000000003</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.376</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.34300000000000003</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.33100000000000002</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.38400000000000001</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.30499999999999999</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.30399999999999999</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.313</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.215</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.19600000000000001</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.18</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.224</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>0.10299999999999999</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.13400000000000001</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.498</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.45600000000000002</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.51600000000000001</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.44800000000000001</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.436</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.41899999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.61099999999999999</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.503</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.53500000000000003</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.628</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.66800000000000004</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.55300000000000005</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.50900000000000001</v>
       </c>
     </row>
@@ -5024,338 +5033,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.13300000000000001</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.104</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.107</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.16400000000000001</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.107</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.10299999999999999</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>0.09</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.216</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.17799999999999999</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.18099999999999999</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.27700000000000002</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.189</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.185</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.13700000000000001</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.105</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.11</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.106</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.10100000000000001</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>0.02</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.19900000000000001</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.16400000000000001</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.13900000000000001</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.14099999999999999</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.23499999999999999</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.155</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.313</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.29199999999999998</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.22900000000000001</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.16400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.17499999999999999</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.152</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.185</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.14099999999999999</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.27700000000000002</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.24099999999999999</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.245</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.28499999999999998</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.22600000000000001</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.219</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.214</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.28799999999999998</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.253</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.25800000000000001</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.30399999999999999</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.23699999999999999</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.23499999999999999</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.151</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.14399999999999999</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.153</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.09</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.38500000000000001</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.33</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.35599999999999998</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.41099999999999998</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.34499999999999997</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.33</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.311</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.49099999999999999</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.36599999999999999</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.40600000000000003</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.54500000000000004</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.45300000000000001</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.4</v>
       </c>
     </row>
@@ -5394,338 +5403,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.189</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.156</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.153</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.22600000000000001</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.15</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.30399999999999999</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.254</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.373</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.25600000000000001</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.247</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.19600000000000001</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.161</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.156</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.23100000000000001</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.15</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.14799999999999999</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>0.04</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.28100000000000003</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.24399999999999999</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.24199999999999999</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.313</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.20100000000000001</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.20699999999999999</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.32700000000000001</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.23899999999999999</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.22700000000000001</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.40699999999999997</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.4</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.30199999999999999</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.23699999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.215</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.187</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.188</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.22500000000000001</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.17899999999999999</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.17199999999999999</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.34499999999999997</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.311</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.34599999999999997</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.27600000000000002</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.26700000000000002</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.27800000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.36099999999999999</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.32800000000000001</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.32</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.37</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.29199999999999998</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.28899999999999998</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.20300000000000001</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.191</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.17399999999999999</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.21199999999999999</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.123</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.158</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.47699999999999998</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.42699999999999999</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.443</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.498</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.43099999999999999</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.41199999999999998</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.39600000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.48399999999999999</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.502</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.61399999999999999</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.53100000000000003</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.48499999999999999</v>
       </c>
     </row>
@@ -5771,20 +5780,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -6490,8 +6499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA134B-6382-4675-9D3B-D18439BEABE0}">
   <dimension ref="B3:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6561,11 +6570,11 @@
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="24"/>
       <c r="D5" s="32">
-        <f t="shared" ref="D5:J5" si="0">(D4-D6)/D4</f>
+        <f>(D4-D6)/D4</f>
         <v>0.2953216374269006</v>
       </c>
       <c r="E5" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D5:J5" si="0">(E4-E6)/E4</f>
         <v>0.34294871794871795</v>
       </c>
       <c r="F5" s="32">
@@ -7012,25 +7021,25 @@
       <c r="C23" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="49">
         <v>20.479099999999999</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="49">
         <v>17.055199999999999</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="49">
         <v>16.732700000000001</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="50">
         <v>23.957100000000001</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="49">
         <v>15.9</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="49">
         <v>15.7637</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="49">
         <v>15.238200000000001</v>
       </c>
     </row>
@@ -7038,28 +7047,28 @@
       <c r="B24" s="41">
         <v>20.446567999999999</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="49">
         <v>5.6402000000000001</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="49">
         <v>4.0423999999999998</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="49">
         <v>5.1342999999999996</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="50">
         <v>7.3920000000000003</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="49">
         <v>4.8</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="49">
         <v>4.5</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="49">
         <v>3.1427999999999998</v>
       </c>
     </row>
@@ -7070,25 +7079,25 @@
       <c r="C25" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="49">
         <v>22.216200000000001</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="49">
         <v>18.7498</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="49">
         <v>18.194600000000001</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="50">
         <v>25.747399999999999</v>
       </c>
-      <c r="H25" s="43">
+      <c r="H25" s="50">
         <v>17.399999999999999</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="49">
         <v>17.494299999999999</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="49">
         <v>17.2562</v>
       </c>
     </row>
@@ -7099,27 +7108,36 @@
       <c r="C26" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="49">
         <v>16.156400000000001</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="49">
         <v>12.839</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="49">
         <v>12.609400000000001</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="50">
         <v>19.9026</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="49">
         <v>13.4</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="49">
         <v>12.5435</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="49">
         <v>11.161300000000001</v>
       </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="41">
@@ -7128,6 +7146,27 @@
       <c r="C28" s="42" t="s">
         <v>86</v>
       </c>
+      <c r="D28" s="49">
+        <v>20.967199999999998</v>
+      </c>
+      <c r="E28" s="49">
+        <v>17.3626</v>
+      </c>
+      <c r="F28" s="49">
+        <v>16.8384</v>
+      </c>
+      <c r="G28" s="50">
+        <v>24.311199999999999</v>
+      </c>
+      <c r="H28" s="49">
+        <v>16.304099999999998</v>
+      </c>
+      <c r="I28" s="49">
+        <v>16.229900000000001</v>
+      </c>
+      <c r="J28" s="49">
+        <v>15.817600000000001</v>
+      </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="41">
@@ -7136,6 +7175,27 @@
       <c r="C29" s="42" t="s">
         <v>87</v>
       </c>
+      <c r="D29" s="49">
+        <v>5.5350000000000001</v>
+      </c>
+      <c r="E29" s="49">
+        <v>3.9685999999999999</v>
+      </c>
+      <c r="F29" s="49">
+        <v>4.7679999999999998</v>
+      </c>
+      <c r="G29" s="49">
+        <v>7.8151999999999999</v>
+      </c>
+      <c r="H29" s="49">
+        <v>5.1481000000000003</v>
+      </c>
+      <c r="I29" s="49">
+        <v>4.8479999999999999</v>
+      </c>
+      <c r="J29" s="49">
+        <v>3.2141000000000002</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="41">
@@ -7144,6 +7204,27 @@
       <c r="C30" s="42" t="s">
         <v>84</v>
       </c>
+      <c r="D30" s="49">
+        <v>22.316600000000001</v>
+      </c>
+      <c r="E30" s="49">
+        <v>18.8017</v>
+      </c>
+      <c r="F30" s="49">
+        <v>18.0425</v>
+      </c>
+      <c r="G30" s="49">
+        <v>25.9008</v>
+      </c>
+      <c r="H30" s="49">
+        <v>17.532900000000001</v>
+      </c>
+      <c r="I30" s="49">
+        <v>17.705200000000001</v>
+      </c>
+      <c r="J30" s="49">
+        <v>17.386399999999998</v>
+      </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="41">
@@ -7152,6 +7233,36 @@
       <c r="C31" s="42" t="s">
         <v>85</v>
       </c>
+      <c r="D31" s="49">
+        <v>16.230499999999999</v>
+      </c>
+      <c r="E31" s="49">
+        <v>13.0413</v>
+      </c>
+      <c r="F31" s="49">
+        <v>12.755100000000001</v>
+      </c>
+      <c r="G31" s="49">
+        <v>20.104679999999998</v>
+      </c>
+      <c r="H31" s="49">
+        <v>13.5511</v>
+      </c>
+      <c r="I31" s="49">
+        <v>12.843299999999999</v>
+      </c>
+      <c r="J31" s="49">
+        <v>11.408200000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="41">
@@ -7160,25 +7271,25 @@
       <c r="C33" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="49">
         <v>19.975300000000001</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="49">
         <v>16.698799999999999</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="49">
         <v>16.102499999999999</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="49">
         <v>23.2</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="49">
         <v>15.216100000000001</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="49">
         <v>15.3818</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="49">
         <v>15.008699999999999</v>
       </c>
     </row>
@@ -7189,25 +7300,25 @@
       <c r="C34" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="49">
         <v>5.8933999999999997</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="49">
         <v>4.1532</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="49">
         <v>5.0208000000000004</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="49">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="49">
         <v>5.2434000000000003</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="49">
         <v>5.3193999999999999</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="49">
         <v>3.4377</v>
       </c>
     </row>
@@ -7218,25 +7329,25 @@
       <c r="C35" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="49">
         <v>21.221800000000002</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="49">
         <v>17.5502</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="49">
         <v>17.078099999999999</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="49">
         <v>17.899999999999999</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="49">
         <v>16.4985</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="49">
         <v>16.534600000000001</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="49">
         <v>15.9984</v>
       </c>
     </row>
@@ -7247,25 +7358,25 @@
       <c r="C36" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="49">
         <v>14.8064</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="49">
         <v>11.4621</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="49">
         <v>11.530099999999999</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="49">
         <v>24.7</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="49">
         <v>11.9268</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="49">
         <v>10.9421</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="49">
         <v>9.8658999999999999</v>
       </c>
     </row>
@@ -7660,338 +7771,338 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.34200000000000003</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.312</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.29499999999999998</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.33600000000000002</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.20200000000000001</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.222</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.28100000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.51600000000000001</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.48499999999999999</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.46</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.51500000000000001</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.34899999999999998</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.371</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.46200000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>0.36</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>0.33200000000000002</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>0.31</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>0.35599999999999998</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>0.20399999999999999</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>0.23200000000000001</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.106</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.06</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.30599999999999999</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.28499999999999998</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.26700000000000002</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.311</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.104</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.16</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.255</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.50700000000000001</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.47199999999999998</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.45700000000000002</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.52</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.38500000000000001</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.378</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.30399999999999999</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.28599999999999998</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.27300000000000002</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.28799999999999998</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.217</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.219</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.25800000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.47099999999999997</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.42699999999999999</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.441</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.33</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.33900000000000002</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.41299999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.48899999999999999</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.47699999999999998</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.442</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.46899999999999997</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>0.34899999999999998</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.36599999999999999</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.224</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.223</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.14699999999999999</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.125</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.17100000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.46</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.44500000000000001</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.41599999999999998</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.48699999999999999</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.26500000000000001</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.34499999999999997</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.44600000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="46">
+      <c r="B15" s="45">
         <v>0.66300000000000003</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="45">
         <v>0.64900000000000002</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="45">
         <v>0.63900000000000001</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="45">
         <v>0.66700000000000004</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="45">
         <v>0.60199999999999998</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="45">
         <v>0.56899999999999995</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="45">
         <v>0.59299999999999997</v>
       </c>
     </row>
@@ -8069,338 +8180,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.24099999999999999</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.19800000000000001</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.26900000000000002</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.18099999999999999</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.187</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>0.192</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.375</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.33100000000000002</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.32</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.435</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.309</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.31900000000000001</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.253</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.216</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.20699999999999999</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.27700000000000002</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.182</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.191</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.19900000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>0.106</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>0.09</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.35599999999999998</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.316</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.314</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.372</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.251</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.26300000000000001</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.26100000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.40699999999999997</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.30599999999999999</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.307</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.495</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.46800000000000003</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.38200000000000001</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.248</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.22700000000000001</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.222</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.251</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.20200000000000001</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.2</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.39600000000000002</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.36799999999999999</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.35499999999999998</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.38300000000000001</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.307</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.31</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.41299999999999998</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.38600000000000001</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.372</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.40899999999999997</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.32500000000000001</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.33300000000000002</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.245</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.23300000000000001</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.20399999999999999</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.246</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>0.114</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.151</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.54200000000000004</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.50900000000000001</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.51100000000000001</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.55100000000000005</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.47899999999999998</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.48199999999999998</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.47099999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.66800000000000004</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.60299999999999998</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.66400000000000003</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.69</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.59499999999999997</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.57799999999999996</v>
       </c>
     </row>
@@ -8439,340 +8550,340 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.13800000000000001</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.106</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.109</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.17199999999999999</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.111</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.106</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.22600000000000001</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.182</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.184</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.19400000000000001</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.19</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.16700000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.14099999999999999</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.108</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.111</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.17399999999999999</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.109</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.105</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>4.7E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>6.3E-2</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.20699999999999999</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.17299999999999999</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.17699999999999999</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.24</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.14499999999999999</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.128</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.25700000000000001</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.157</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.16900000000000001</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.33300000000000002</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.31900000000000001</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.17699999999999999</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.14899999999999999</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.156</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.188</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.152</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.14399999999999999</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.28199999999999997</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.24399999999999999</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.251</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.29099999999999998</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.23100000000000001</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.221</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.214</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.29499999999999998</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.25700000000000001</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.311</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.24199999999999999</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.22900000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.156</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.156</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.39200000000000002</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.34399999999999997</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.36499999999999999</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.42</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.35399999999999998</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.33800000000000002</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.495</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.38</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.42399999999999999</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.55700000000000005</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.47499999999999998</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.41399999999999998</v>
       </c>
     </row>
@@ -8811,338 +8922,338 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>0.20499999999999999</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>0.16800000000000001</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>0.16600000000000001</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>0.24</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>0.16300000000000001</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>0.159</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>0.153</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>0.32400000000000001</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>0.27700000000000002</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>0.27200000000000002</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>0.39200000000000002</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>0.27900000000000003</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>0.27500000000000002</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>0.26900000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>0.215</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.17299999999999999</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>0.17199999999999999</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>0.248</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>0.16200000000000001</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.153</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>3.1E-2</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>0.30099999999999999</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>0.33300000000000002</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>0.219</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>0.222</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>0.35399999999999998</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>0.24199999999999999</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>0.25600000000000001</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>0.44900000000000001</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>0.433</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>0.223</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>0.193</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>0.19500000000000001</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>0.187</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>0.182</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>0.182</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>0.35799999999999998</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>0.32300000000000001</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>0.316</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>0.35699999999999998</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.28499999999999998</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>0.375</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>0.34</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="45">
         <v>0.33300000000000002</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>0.38100000000000001</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <v>0.30099999999999999</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="45">
         <v>0.30199999999999999</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>0.312</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>0.21199999999999999</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="45">
         <v>0.19900000000000001</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="45">
         <v>0.184</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>0.22</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>0.10100000000000001</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>0.13200000000000001</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.158</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>0.495</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>0.45200000000000001</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>0.45400000000000001</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>0.51200000000000001</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>0.44500000000000001</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="45">
         <v>0.433</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>0.41699999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>0.625</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>0.5</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0.54100000000000004</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>0.63800000000000001</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>0.65200000000000002</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <v>0.55200000000000005</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>0.53300000000000003</v>
       </c>
     </row>

</xml_diff>